<commit_message>
Gantt Chard is updated.
</commit_message>
<xml_diff>
--- a/Course Materials/Gantt Chard.xlsx
+++ b/Course Materials/Gantt Chard.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>PERIODS</t>
   </si>
@@ -682,20 +682,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1109,7 +1109,7 @@
   <dimension ref="A2:AB30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="61" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AU8" sqref="AU8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="38">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H3" s="30"/>
       <c r="I3" s="7" t="s">
@@ -1201,22 +1201,22 @@
     </row>
     <row r="4" spans="1:28" s="5" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35"/>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="44" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="14" t="s">
@@ -1239,12 +1239,12 @@
     </row>
     <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
       <c r="H5" s="36">
         <v>1</v>
       </c>
@@ -1433,11 +1433,11 @@
       <c r="E9" s="25">
         <v>6</v>
       </c>
-      <c r="F9" s="29" t="s">
-        <v>18</v>
+      <c r="F9" s="29">
+        <v>2</v>
       </c>
       <c r="G9" s="26">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H9" s="40"/>
       <c r="I9" s="18"/>
@@ -1462,19 +1462,19 @@
     </row>
     <row r="10" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="24"/>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="42">
         <v>6</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="42">
         <v>1</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="41">
         <v>6</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="41">
         <v>1</v>
       </c>
       <c r="G10" s="26">
@@ -1512,14 +1512,14 @@
       <c r="D11" s="25">
         <v>2</v>
       </c>
-      <c r="E11" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>18</v>
+      <c r="E11" s="29">
+        <v>7</v>
+      </c>
+      <c r="F11" s="29">
+        <v>2</v>
       </c>
       <c r="G11" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="40"/>
       <c r="I11" s="18"/>
@@ -1553,14 +1553,14 @@
       <c r="D12" s="25">
         <v>1</v>
       </c>
-      <c r="E12" s="29" t="s">
-        <v>18</v>
+      <c r="E12" s="29">
+        <v>8</v>
       </c>
       <c r="F12" s="29" t="s">
         <v>18</v>
       </c>
       <c r="G12" s="26">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H12" s="40"/>
       <c r="I12" s="18"/>

</xml_diff>

<commit_message>
Fuselage internal structure is modified.
</commit_message>
<xml_diff>
--- a/Course Materials/Gantt Chard.xlsx
+++ b/Course Materials/Gantt Chard.xlsx
@@ -1108,8 +1108,8 @@
   </sheetPr>
   <dimension ref="A2:AB30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="61" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="61" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1560,7 +1560,7 @@
         <v>18</v>
       </c>
       <c r="G12" s="26">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="H12" s="40"/>
       <c r="I12" s="18"/>

</xml_diff>

<commit_message>
Gantt chars are updated and desgin path is added.
</commit_message>
<xml_diff>
--- a/Course Materials/Gantt Chard.xlsx
+++ b/Course Materials/Gantt Chard.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>PERIODS</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>Airfoil Selection</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Conceptual Design Research</t>
@@ -558,7 +555,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -618,9 +615,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1108,8 +1102,8 @@
   </sheetPr>
   <dimension ref="A2:AB30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="61" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="61" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1129,7 +1123,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="1">
-      <c r="A2" s="24"/>
+      <c r="A2" s="23"/>
       <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
@@ -1155,8 +1149,8 @@
       <c r="V2" s="11"/>
     </row>
     <row r="3" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
-      <c r="B3" s="21" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="12"/>
@@ -1165,29 +1159,29 @@
         <v>3</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="38">
-        <v>9</v>
-      </c>
-      <c r="H3" s="30"/>
+      <c r="G3" s="37">
+        <v>15</v>
+      </c>
+      <c r="H3" s="29"/>
       <c r="I3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="J3" s="7"/>
-      <c r="K3" s="31"/>
+      <c r="K3" s="30"/>
       <c r="L3" s="7" t="s">
         <v>9</v>
       </c>
       <c r="M3" s="7"/>
-      <c r="N3" s="32"/>
+      <c r="N3" s="31"/>
       <c r="O3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="P3" s="6"/>
-      <c r="Q3" s="33"/>
+      <c r="Q3" s="32"/>
       <c r="R3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="34"/>
+      <c r="S3" s="33"/>
       <c r="T3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1200,23 +1194,23 @@
       <c r="AB3" s="6"/>
     </row>
     <row r="4" spans="1:28" s="5" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
-      <c r="B4" s="45" t="s">
+      <c r="A4" s="34"/>
+      <c r="B4" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="44" t="s">
+      <c r="G4" s="43" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="14" t="s">
@@ -1238,56 +1232,56 @@
       <c r="V4" s="17"/>
     </row>
     <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="36">
-        <v>1</v>
-      </c>
-      <c r="I5" s="36">
+      <c r="A5" s="23"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="35">
+        <v>1</v>
+      </c>
+      <c r="I5" s="35">
         <v>2</v>
       </c>
-      <c r="J5" s="36">
+      <c r="J5" s="35">
         <v>3</v>
       </c>
-      <c r="K5" s="36">
+      <c r="K5" s="35">
         <v>4</v>
       </c>
-      <c r="L5" s="36">
+      <c r="L5" s="35">
         <v>5</v>
       </c>
-      <c r="M5" s="36">
+      <c r="M5" s="35">
         <v>6</v>
       </c>
-      <c r="N5" s="36">
+      <c r="N5" s="35">
         <v>7</v>
       </c>
-      <c r="O5" s="36">
+      <c r="O5" s="35">
         <v>8</v>
       </c>
-      <c r="P5" s="36">
+      <c r="P5" s="35">
         <v>9</v>
       </c>
-      <c r="Q5" s="36">
+      <c r="Q5" s="35">
         <v>10</v>
       </c>
-      <c r="R5" s="36">
+      <c r="R5" s="35">
         <v>11</v>
       </c>
-      <c r="S5" s="36">
+      <c r="S5" s="35">
         <v>12</v>
       </c>
-      <c r="T5" s="36">
+      <c r="T5" s="35">
         <v>13</v>
       </c>
-      <c r="U5" s="36">
+      <c r="U5" s="35">
         <v>14</v>
       </c>
-      <c r="V5" s="37">
+      <c r="V5" s="36">
         <v>15</v>
       </c>
       <c r="W5"/>
@@ -1297,26 +1291,26 @@
       <c r="AA5"/>
     </row>
     <row r="6" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24"/>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="23"/>
+      <c r="B6" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="25">
-        <v>1</v>
-      </c>
-      <c r="D6" s="25">
+      <c r="C6" s="24">
+        <v>1</v>
+      </c>
+      <c r="D6" s="24">
         <v>4</v>
       </c>
-      <c r="E6" s="25">
-        <v>1</v>
-      </c>
-      <c r="F6" s="25">
+      <c r="E6" s="24">
+        <v>1</v>
+      </c>
+      <c r="F6" s="24">
         <v>4</v>
       </c>
-      <c r="G6" s="26">
-        <v>1</v>
-      </c>
-      <c r="H6" s="39"/>
+      <c r="G6" s="25">
+        <v>1</v>
+      </c>
+      <c r="H6" s="38"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -1338,26 +1332,26 @@
       <c r="AA6"/>
     </row>
     <row r="7" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="24">
         <v>4</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="24">
         <v>2</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="24">
         <v>4</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="24">
         <v>2</v>
       </c>
-      <c r="G7" s="26">
-        <v>1</v>
-      </c>
-      <c r="H7" s="40"/>
+      <c r="G7" s="25">
+        <v>1</v>
+      </c>
+      <c r="H7" s="39"/>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
@@ -1379,26 +1373,26 @@
       <c r="AA7"/>
     </row>
     <row r="8" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24"/>
-      <c r="B8" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="25">
+      <c r="A8" s="23"/>
+      <c r="B8" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="24">
         <v>5</v>
       </c>
-      <c r="D8" s="25">
-        <v>1</v>
-      </c>
-      <c r="E8" s="25">
+      <c r="D8" s="24">
+        <v>1</v>
+      </c>
+      <c r="E8" s="24">
         <v>5</v>
       </c>
-      <c r="F8" s="29">
-        <v>1</v>
-      </c>
-      <c r="G8" s="26">
-        <v>1</v>
-      </c>
-      <c r="H8" s="40"/>
+      <c r="F8" s="28">
+        <v>1</v>
+      </c>
+      <c r="G8" s="25">
+        <v>1</v>
+      </c>
+      <c r="H8" s="39"/>
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
       <c r="K8" s="18"/>
@@ -1420,26 +1414,26 @@
       <c r="AA8"/>
     </row>
     <row r="9" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="23" t="s">
+      <c r="A9" s="23"/>
+      <c r="B9" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="24">
         <v>6</v>
       </c>
-      <c r="D9" s="25">
-        <v>1</v>
-      </c>
-      <c r="E9" s="25">
+      <c r="D9" s="24">
+        <v>1</v>
+      </c>
+      <c r="E9" s="24">
         <v>6</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="28">
         <v>2</v>
       </c>
-      <c r="G9" s="26">
-        <v>1</v>
-      </c>
-      <c r="H9" s="40"/>
+      <c r="G9" s="25">
+        <v>1</v>
+      </c>
+      <c r="H9" s="39"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
@@ -1461,26 +1455,26 @@
       <c r="AA9"/>
     </row>
     <row r="10" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
-      <c r="B10" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="42">
+      <c r="A10" s="23"/>
+      <c r="B10" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="41">
         <v>6</v>
       </c>
-      <c r="D10" s="42">
-        <v>1</v>
-      </c>
-      <c r="E10" s="41">
+      <c r="D10" s="41">
+        <v>1</v>
+      </c>
+      <c r="E10" s="40">
         <v>6</v>
       </c>
-      <c r="F10" s="41">
-        <v>1</v>
-      </c>
-      <c r="G10" s="26">
-        <v>1</v>
-      </c>
-      <c r="H10" s="40"/>
+      <c r="F10" s="40">
+        <v>1</v>
+      </c>
+      <c r="G10" s="25">
+        <v>1</v>
+      </c>
+      <c r="H10" s="39"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
@@ -1502,26 +1496,26 @@
       <c r="AA10"/>
     </row>
     <row r="11" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24"/>
-      <c r="B11" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="25">
+      <c r="A11" s="23"/>
+      <c r="B11" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="24">
         <v>7</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="24">
         <v>2</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="28">
         <v>7</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="28">
         <v>2</v>
       </c>
-      <c r="G11" s="26">
-        <v>1</v>
-      </c>
-      <c r="H11" s="40"/>
+      <c r="G11" s="25">
+        <v>1</v>
+      </c>
+      <c r="H11" s="39"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
@@ -1543,26 +1537,26 @@
       <c r="AA11"/>
     </row>
     <row r="12" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="24">
         <v>8</v>
       </c>
-      <c r="D12" s="25">
-        <v>1</v>
-      </c>
-      <c r="E12" s="29">
+      <c r="D12" s="24">
+        <v>1</v>
+      </c>
+      <c r="E12" s="28">
         <v>8</v>
       </c>
-      <c r="F12" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="26">
-        <v>0.5</v>
-      </c>
-      <c r="H12" s="40"/>
+      <c r="F12" s="28">
+        <v>1</v>
+      </c>
+      <c r="G12" s="25">
+        <v>1</v>
+      </c>
+      <c r="H12" s="39"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
@@ -1584,26 +1578,26 @@
       <c r="AA12"/>
     </row>
     <row r="13" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="25">
+      <c r="A13" s="23"/>
+      <c r="B13" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="24">
         <v>9</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="24">
         <v>3</v>
       </c>
-      <c r="E13" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="26">
-        <v>0</v>
-      </c>
-      <c r="H13" s="40"/>
+      <c r="E13" s="28">
+        <v>9</v>
+      </c>
+      <c r="F13" s="28">
+        <v>3</v>
+      </c>
+      <c r="G13" s="25">
+        <v>1</v>
+      </c>
+      <c r="H13" s="39"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
@@ -1625,26 +1619,26 @@
       <c r="AA13"/>
     </row>
     <row r="14" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
-      <c r="B14" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="25">
+      <c r="A14" s="23"/>
+      <c r="B14" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="24">
         <v>10</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="24">
         <v>2</v>
       </c>
-      <c r="E14" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="26">
-        <v>0</v>
-      </c>
-      <c r="H14" s="40"/>
+      <c r="E14" s="28">
+        <v>10</v>
+      </c>
+      <c r="F14" s="28">
+        <v>3</v>
+      </c>
+      <c r="G14" s="25">
+        <v>1</v>
+      </c>
+      <c r="H14" s="39"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="18"/>
@@ -1666,26 +1660,26 @@
       <c r="AA14"/>
     </row>
     <row r="15" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
-      <c r="B15" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="24">
         <v>11</v>
       </c>
-      <c r="D15" s="25">
-        <v>1</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="26">
-        <v>0</v>
-      </c>
-      <c r="H15" s="40"/>
+      <c r="D15" s="24">
+        <v>1</v>
+      </c>
+      <c r="E15" s="28">
+        <v>11</v>
+      </c>
+      <c r="F15" s="28">
+        <v>1</v>
+      </c>
+      <c r="G15" s="25">
+        <v>1</v>
+      </c>
+      <c r="H15" s="39"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
@@ -1707,26 +1701,26 @@
       <c r="AA15"/>
     </row>
     <row r="16" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="24"/>
-      <c r="B16" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="24">
         <v>11</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="24">
         <v>2</v>
       </c>
-      <c r="E16" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="26">
-        <v>0</v>
-      </c>
-      <c r="H16" s="40"/>
+      <c r="E16" s="28">
+        <v>11</v>
+      </c>
+      <c r="F16" s="28">
+        <v>2</v>
+      </c>
+      <c r="G16" s="25">
+        <v>1</v>
+      </c>
+      <c r="H16" s="39"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
@@ -1748,26 +1742,26 @@
       <c r="AA16"/>
     </row>
     <row r="17" spans="1:27" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="24"/>
-      <c r="B17" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="27">
+      <c r="A17" s="23"/>
+      <c r="B17" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="26">
         <v>12</v>
       </c>
-      <c r="D17" s="25">
-        <v>1</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="26">
-        <v>0</v>
-      </c>
-      <c r="H17" s="40"/>
+      <c r="D17" s="24">
+        <v>1</v>
+      </c>
+      <c r="E17" s="28">
+        <v>12</v>
+      </c>
+      <c r="F17" s="28">
+        <v>2</v>
+      </c>
+      <c r="G17" s="25">
+        <v>1</v>
+      </c>
+      <c r="H17" s="39"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
@@ -1789,26 +1783,26 @@
       <c r="AA17"/>
     </row>
     <row r="18" spans="1:27" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="25">
+      <c r="A18" s="23"/>
+      <c r="B18" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="24">
         <v>13</v>
       </c>
-      <c r="D18" s="25">
-        <v>1</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="26">
-        <v>0</v>
-      </c>
-      <c r="H18" s="40"/>
+      <c r="D18" s="24">
+        <v>1</v>
+      </c>
+      <c r="E18" s="28">
+        <v>13</v>
+      </c>
+      <c r="F18" s="28">
+        <v>1</v>
+      </c>
+      <c r="G18" s="25">
+        <v>1</v>
+      </c>
+      <c r="H18" s="39"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
@@ -1830,25 +1824,25 @@
       <c r="AA18"/>
     </row>
     <row r="19" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="25">
+      <c r="B19" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="24">
         <v>13</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="24">
         <v>3</v>
       </c>
-      <c r="E19" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="20">
-        <v>0</v>
-      </c>
-      <c r="H19" s="40"/>
+      <c r="E19" s="27">
+        <v>13</v>
+      </c>
+      <c r="F19" s="27">
+        <v>3</v>
+      </c>
+      <c r="G19" s="25">
+        <v>1</v>
+      </c>
+      <c r="H19" s="39"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>

</xml_diff>